<commit_message>
tried and added xgboost and random forest
</commit_message>
<xml_diff>
--- a/records/predictionNotes.xlsx
+++ b/records/predictionNotes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>approach_id</t>
   </si>
@@ -139,9 +139,6 @@
     <t>curves look good, look in plots/ directory</t>
   </si>
   <si>
-    <t>have to check with news / media the next 10 days, not much utility without that</t>
-  </si>
-  <si>
     <t>projection.csv (worldometers.info manual fetch)</t>
   </si>
   <si>
@@ -149,6 +146,24 @@
   </si>
   <si>
     <t>terrible fit, need to upgrade to polynomial regression</t>
+  </si>
+  <si>
+    <t>RandomForestRegressor(max_depth=5, random_state=12, n_estimators=250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">significantly improves over polynomial regression </t>
+  </si>
+  <si>
+    <t>PolynomialFeatures between 2 and 6 (depending upon data length) works best</t>
+  </si>
+  <si>
+    <t>xgboost</t>
+  </si>
+  <si>
+    <t>slightly improves over random forest</t>
+  </si>
+  <si>
+    <t>the zoomed in fit is a lot better but train/test split doesn't work as good but can be parameterized better</t>
   </si>
 </sst>
 </file>
@@ -489,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,7 +520,7 @@
     <col min="6" max="6" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="124.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -671,7 +686,7 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
@@ -683,7 +698,7 @@
         <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -703,7 +718,7 @@
         <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -723,7 +738,47 @@
         <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated healthy people and cleaned individiualdetails (stored in custom_confirmed)
</commit_message>
<xml_diff>
--- a/records/predictionNotes.xlsx
+++ b/records/predictionNotes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>approach_id</t>
   </si>
@@ -151,19 +151,22 @@
     <t>RandomForestRegressor(max_depth=5, random_state=12, n_estimators=250)</t>
   </si>
   <si>
-    <t xml:space="preserve">significantly improves over polynomial regression </t>
-  </si>
-  <si>
     <t>PolynomialFeatures between 2 and 6 (depending upon data length) works best</t>
   </si>
   <si>
     <t>xgboost</t>
   </si>
   <si>
-    <t>slightly improves over random forest</t>
-  </si>
-  <si>
     <t>the zoomed in fit is a lot better but train/test split doesn't work as good but can be parameterized better</t>
+  </si>
+  <si>
+    <t>slightly improves over random forest | UPDATE: same as above</t>
+  </si>
+  <si>
+    <t>significantly improves over polynomial regression | UPDATE: it doesn't actually improve anything, tree based methods are not for time series predictions, i.e they don’t perform well oustide training boundaries; Try something else.</t>
+  </si>
+  <si>
+    <t>cancelled (see update)</t>
   </si>
 </sst>
 </file>
@@ -506,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -738,10 +741,13 @@
         <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" t="s">
         <v>30</v>
       </c>
@@ -755,15 +761,18 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -778,7 +787,7 @@
         <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
performed various binary classification algorithms
</commit_message>
<xml_diff>
--- a/records/predictionNotes.xlsx
+++ b/records/predictionNotes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>approach_id</t>
   </si>
@@ -167,6 +167,78 @@
   </si>
   <si>
     <t>cancelled (see update)</t>
+  </si>
+  <si>
+    <t>trying binary classification on custom datasets</t>
+  </si>
+  <si>
+    <t>custom_confirmed and custom_ healthy</t>
+  </si>
+  <si>
+    <t>built these two datasets by cleaning IndividualDetails.csv and india_age_groups_city.xls (census age group data by city) details in ipynb</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>accuracy obtained: 86.04%</t>
+  </si>
+  <si>
+    <t>MLPC</t>
+  </si>
+  <si>
+    <t>accuracy obtained: 86.14%</t>
+  </si>
+  <si>
+    <t>not bad, pretty consistent</t>
+  </si>
+  <si>
+    <t>very unreliable, dropped to 65% one time on the exact same train/test split</t>
+  </si>
+  <si>
+    <t>accuracy obtained: ~65% - 86.14%</t>
+  </si>
+  <si>
+    <t>SVM (linear one v all)</t>
+  </si>
+  <si>
+    <t>SVM (multiclass)</t>
+  </si>
+  <si>
+    <t>consistent</t>
+  </si>
+  <si>
+    <t>consistent, not very different from one vs all</t>
+  </si>
+  <si>
+    <t>do, very similar to one vs all</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>accuracy obtained: 93.49%</t>
+  </si>
+  <si>
+    <t>best yet, tried a n_neighbors parameter of 2</t>
+  </si>
+  <si>
+    <t>decision tree</t>
+  </si>
+  <si>
+    <t>accuracy obtained: 92.51%</t>
+  </si>
+  <si>
+    <t>consistent; same score with crossvalidation</t>
+  </si>
+  <si>
+    <t>do + crossval</t>
+  </si>
+  <si>
+    <t>accuracy obtained: 99.32%</t>
+  </si>
+  <si>
+    <t>not sure if I did it the correct way. [?] question about crossvalidation, if I DID, result is brilliant.</t>
   </si>
 </sst>
 </file>
@@ -507,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -790,6 +862,149 @@
         <v>47</v>
       </c>
     </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>4.2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8">
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>